<commit_message>
Switching to VLJ # in the spreadsheet
</commit_message>
<xml_diff>
--- a/spec/support/blankJudgeSpreadsheet.xlsx
+++ b/spec/support/blankJudgeSpreadsheet.xlsx
@@ -19,7 +19,7 @@
     <t>Judge Name</t>
   </si>
   <si>
-    <t>CSS Id</t>
+    <t>VLJ #</t>
   </si>
   <si>
     <t>Date</t>
@@ -31,7 +31,7 @@
     <t>Jones, Bernard</t>
   </si>
   <si>
-    <t>BVAJONESB</t>
+    <t>123</t>
   </si>
 </sst>
 </file>
@@ -50,7 +50,7 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="Helvetica"/>
     </font>
     <font>
       <sz val="15"/>
@@ -105,7 +105,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -382,13 +382,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -398,19 +440,19 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -422,10 +464,10 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -446,7 +488,7 @@
     <xf numFmtId="14" fontId="6" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -458,10 +500,10 @@
     <xf numFmtId="14" fontId="6" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -473,16 +515,34 @@
     <xf numFmtId="14" fontId="6" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -555,14 +615,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office Theme">
       <a:majorFont>
-        <a:latin typeface="Helvetica Neue"/>
-        <a:ea typeface="Helvetica Neue"/>
-        <a:cs typeface="Helvetica Neue"/>
+        <a:latin typeface="Helvetica"/>
+        <a:ea typeface="Helvetica"/>
+        <a:cs typeface="Helvetica"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Helvetica Neue"/>
-        <a:ea typeface="Helvetica Neue"/>
-        <a:cs typeface="Helvetica Neue"/>
+        <a:latin typeface="Helvetica"/>
+        <a:ea typeface="Helvetica"/>
+        <a:cs typeface="Helvetica"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office Theme">
@@ -767,10 +827,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica"/>
-            <a:ea typeface="Helvetica"/>
-            <a:cs typeface="Helvetica"/>
-            <a:sym typeface="Helvetica"/>
+            <a:latin typeface="Helvetica Neue"/>
+            <a:ea typeface="Helvetica Neue"/>
+            <a:cs typeface="Helvetica Neue"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1344,10 +1404,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica"/>
-            <a:ea typeface="Helvetica"/>
-            <a:cs typeface="Helvetica"/>
-            <a:sym typeface="Helvetica"/>
+            <a:latin typeface="Helvetica Neue"/>
+            <a:ea typeface="Helvetica Neue"/>
+            <a:cs typeface="Helvetica Neue"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1598,18 +1658,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.8672" style="1" customWidth="1"/>
     <col min="2" max="2" width="29" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.8516" style="1" customWidth="1"/>
-    <col min="5" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.8516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7344" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.8672" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.8672" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
     <col min="10" max="256" width="11" style="1" customWidth="1"/>
   </cols>
@@ -1742,6 +1804,28 @@
       <c r="H8" s="30"/>
       <c r="I8" s="31"/>
     </row>
+    <row r="9" ht="17" customHeight="1">
+      <c r="A9" s="32"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="34"/>
+    </row>
+    <row r="10" ht="17" customHeight="1">
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="37"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
@@ -1749,7 +1833,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
VLJ # in spreadsheet instead of css_id (#6460)
</commit_message>
<xml_diff>
--- a/spec/support/blankJudgeSpreadsheet.xlsx
+++ b/spec/support/blankJudgeSpreadsheet.xlsx
@@ -19,7 +19,7 @@
     <t>Judge Name</t>
   </si>
   <si>
-    <t>CSS Id</t>
+    <t>VLJ #</t>
   </si>
   <si>
     <t>Date</t>
@@ -31,7 +31,7 @@
     <t>Jones, Bernard</t>
   </si>
   <si>
-    <t>BVAJONESB</t>
+    <t>123</t>
   </si>
 </sst>
 </file>
@@ -50,7 +50,7 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="Helvetica"/>
     </font>
     <font>
       <sz val="15"/>
@@ -105,7 +105,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -382,13 +382,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -398,19 +440,19 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -422,10 +464,10 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -446,7 +488,7 @@
     <xf numFmtId="14" fontId="6" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -458,10 +500,10 @@
     <xf numFmtId="14" fontId="6" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -473,16 +515,34 @@
     <xf numFmtId="14" fontId="6" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -555,14 +615,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office Theme">
       <a:majorFont>
-        <a:latin typeface="Helvetica Neue"/>
-        <a:ea typeface="Helvetica Neue"/>
-        <a:cs typeface="Helvetica Neue"/>
+        <a:latin typeface="Helvetica"/>
+        <a:ea typeface="Helvetica"/>
+        <a:cs typeface="Helvetica"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Helvetica Neue"/>
-        <a:ea typeface="Helvetica Neue"/>
-        <a:cs typeface="Helvetica Neue"/>
+        <a:latin typeface="Helvetica"/>
+        <a:ea typeface="Helvetica"/>
+        <a:cs typeface="Helvetica"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office Theme">
@@ -767,10 +827,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica"/>
-            <a:ea typeface="Helvetica"/>
-            <a:cs typeface="Helvetica"/>
-            <a:sym typeface="Helvetica"/>
+            <a:latin typeface="Helvetica Neue"/>
+            <a:ea typeface="Helvetica Neue"/>
+            <a:cs typeface="Helvetica Neue"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1344,10 +1404,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica"/>
-            <a:ea typeface="Helvetica"/>
-            <a:cs typeface="Helvetica"/>
-            <a:sym typeface="Helvetica"/>
+            <a:latin typeface="Helvetica Neue"/>
+            <a:ea typeface="Helvetica Neue"/>
+            <a:cs typeface="Helvetica Neue"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1598,18 +1658,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.8672" style="1" customWidth="1"/>
     <col min="2" max="2" width="29" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.8516" style="1" customWidth="1"/>
-    <col min="5" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.8516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7344" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.8672" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.8672" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
     <col min="10" max="256" width="11" style="1" customWidth="1"/>
   </cols>
@@ -1742,6 +1804,28 @@
       <c r="H8" s="30"/>
       <c r="I8" s="31"/>
     </row>
+    <row r="9" ht="17" customHeight="1">
+      <c r="A9" s="32"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="34"/>
+    </row>
+    <row r="10" ht="17" customHeight="1">
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="37"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
@@ -1749,7 +1833,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>